<commit_message>
Labels - Manual Done
</commit_message>
<xml_diff>
--- a/Capstone Report.xlsx
+++ b/Capstone Report.xlsx
@@ -8,16 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isalau/Documents/GitHub/Coursera_Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DF9FE8-753B-9E4A-B633-9C98DEF29E3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68410BC4-2DA5-764A-AC3F-C76AAFE3C058}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="1" xr2:uid="{96F98A8C-62FC-DE48-AC03-E5AB07280DC8}"/>
+    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{96F98A8C-62FC-DE48-AC03-E5AB07280DC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Neighborhoods A.1" sheetId="1" r:id="rId1"/>
     <sheet name="Venues" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId3"/>
+    <sheet name="Venues (2)" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$A$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Venues!#REF!</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Venues (2)'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="455">
   <si>
     <t>Longitude</t>
   </si>
@@ -1388,6 +1392,66 @@
   </si>
   <si>
     <t>Residential/Toursim</t>
+  </si>
+  <si>
+    <t>Bakery	Bagel Shop	Chocolate Shop	Convenience Store	Cupcake Shop	Deli / Bodega	Dessert Shop	Donut Shop	Drugstore	Farmers Market	Food	Food &amp; Drink Shop	Gourmet Shop	Grocery Store	Liquor Store	Market	Organic Grocery	Pharmacy	Smoothie Shop	Snack Place	Supermarket	Supplement Shop	Wine Shop	Beer Store</t>
+  </si>
+  <si>
+    <t>Chiropractor
+Health &amp; Beauty Service
+Hospital
+Massage Studio
+Nail Salon
+Spa
+Salon / Barbershop</t>
+  </si>
+  <si>
+    <t>Dog Run
+Dry Cleaner
+Home Service
+Laundromat
+Locksmith
+Moving Target
+Other Repair Shop
+Pet Service
+Shoe Repair
+Storage Facility
+Tailor Shop
+Residential Building (Apartment / Condo)</t>
+  </si>
+  <si>
+    <t>Athletics &amp; Sports
+Baseball Field
+Basketball Court
+Basketball Stadium
+Boxing Gym
+Cycle Studio
+Dance Studio
+Field
+Golf Course
+Gym
+Gym / Fitness Center
+Gym Pool
+Gymnastics Gym
+Harbor / Marina
+Heliport
+Lake
+Martial Arts School
+Pilates Studio
+Playground
+Skating Rink
+Soccer Field
+Soccer Stadium
+Sports Club
+State / Provincial Park
+Volleyball Court
+Yoga Studio
+Recreation Center
+Track
+Tennis Court</t>
+  </si>
+  <si>
+    <t>Afghan Restaurant',</t>
   </si>
 </sst>
 </file>
@@ -1445,13 +1509,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3252,9 +3320,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6CA468-A613-9049-8123-A1A938CC80B4}">
   <dimension ref="A1:S81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4064,7 +4132,7 @@
         <v>230</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -4079,10 +4147,13 @@
         <v>232</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="D31" s="1" t="s">
+        <v>406</v>
+      </c>
       <c r="F31" s="1" t="s">
         <v>314</v>
       </c>
@@ -4091,7 +4162,7 @@
         <v>233</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>401</v>
+        <v>371</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -4103,7 +4174,7 @@
         <v>238</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -4151,9 +4222,6 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.2">
@@ -4438,8 +4506,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G3:G101">
-    <sortCondition ref="G3:G101"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I3:I36">
+    <sortCondition ref="I36"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="Q1:S1"/>
@@ -4449,4 +4517,1505 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D9AED1F-375D-ED42-8CBE-71E49D33018F}">
+  <dimension ref="A1:A79"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A69" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A71" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B100DFC4-B92D-BB4D-A28B-775CD5752A38}">
+  <dimension ref="A1:X90"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S3" sqref="S3:S8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" customWidth="1"/>
+    <col min="8" max="8" width="38.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="37.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="F1" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="N1" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="O1" s="3"/>
+      <c r="Q1" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>446</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="Q7" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q9" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q10" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="Q11" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="18" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="F17" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="F19" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="F23" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="F25" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="F26" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="D27" s="1"/>
+      <c r="F27" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="D28" s="1"/>
+      <c r="F28" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="F29" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="D30" s="1"/>
+      <c r="F30" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="D31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F32" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+      <c r="F33" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F34" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F35" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A36" s="1"/>
+      <c r="F36" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F37" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F38" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F39" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F40" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F41" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F42" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F43" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F44" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F45" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F46" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F47" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="F48" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="F49" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="F50" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H52" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H53" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H54" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H55" s="1" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H56" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H57" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H58" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A59" s="1"/>
+      <c r="H59" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H61" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H62" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H63" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H64" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H65" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H66" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="G67" s="1"/>
+      <c r="H67" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H68" s="1" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H69" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A70" s="1"/>
+      <c r="H70" s="1" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H71" s="1" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H72" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H73" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H74" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H75" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H76" s="1" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="G77" s="1"/>
+      <c r="H77" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H78" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H79" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="H80" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="81" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="H81" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="90" spans="1:24" ht="18" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1"/>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+      <c r="R90" s="1"/>
+      <c r="S90" s="1"/>
+      <c r="T90" s="1"/>
+      <c r="U90" s="1"/>
+      <c r="V90" s="1"/>
+      <c r="W90" s="1"/>
+      <c r="X90" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:S1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>